<commit_message>
Updated CSV and URL
</commit_message>
<xml_diff>
--- a/data/ExchangeRate.xlsx
+++ b/data/ExchangeRate.xlsx
@@ -5,46 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dlnphng/Documents/FIT3179/Week10/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dlnphng/Documents/FIT3179/A2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7280D70F-3388-3349-B7F7-B2313E638D8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5974FD25-4015-1742-B154-ADBD6F6AE000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="560" windowWidth="19280" windowHeight="14520" xr2:uid="{8F6BB1B3-1D13-4443-AAE2-9163E16F6751}"/>
+    <workbookView xWindow="60" yWindow="560" windowWidth="28740" windowHeight="14520" xr2:uid="{8F6BB1B3-1D13-4443-AAE2-9163E16F6751}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$2:$A$121</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$B$2:$B$121</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$C$2:$C$121</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$A$2:$A$121</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$B$2:$B$121</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$C$2:$C$121</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Sheet1!$A$2:$A$121</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$2:$B$121</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">Sheet1!$B$2:$B$121</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">Sheet1!$C$2:$C$121</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">Sheet1!$A$2:$A$121</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">Sheet1!$B$2:$B$121</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">Sheet1!$C$2:$C$121</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$A$2:$A$121</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$B$2:$B$121</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$C$2:$C$121</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$A$2:$A$121</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$B$1</definedName>
-  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -66,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="123">
   <si>
     <t>Time</t>
   </si>
@@ -75,6 +45,366 @@
   </si>
   <si>
     <t>Exchange rates</t>
+  </si>
+  <si>
+    <t>2010-01</t>
+  </si>
+  <si>
+    <t>2010-02</t>
+  </si>
+  <si>
+    <t>2010-03</t>
+  </si>
+  <si>
+    <t>2010-04</t>
+  </si>
+  <si>
+    <t>2010-05</t>
+  </si>
+  <si>
+    <t>2010-06</t>
+  </si>
+  <si>
+    <t>2010-07</t>
+  </si>
+  <si>
+    <t>2010-08</t>
+  </si>
+  <si>
+    <t>2010-09</t>
+  </si>
+  <si>
+    <t>2010-10</t>
+  </si>
+  <si>
+    <t>2010-11</t>
+  </si>
+  <si>
+    <t>2010-12</t>
+  </si>
+  <si>
+    <t>2011-01</t>
+  </si>
+  <si>
+    <t>2011-02</t>
+  </si>
+  <si>
+    <t>2011-03</t>
+  </si>
+  <si>
+    <t>2011-04</t>
+  </si>
+  <si>
+    <t>2011-05</t>
+  </si>
+  <si>
+    <t>2011-06</t>
+  </si>
+  <si>
+    <t>2011-07</t>
+  </si>
+  <si>
+    <t>2011-08</t>
+  </si>
+  <si>
+    <t>2011-09</t>
+  </si>
+  <si>
+    <t>2011-10</t>
+  </si>
+  <si>
+    <t>2011-11</t>
+  </si>
+  <si>
+    <t>2011-12</t>
+  </si>
+  <si>
+    <t>2012-01</t>
+  </si>
+  <si>
+    <t>2012-02</t>
+  </si>
+  <si>
+    <t>2012-03</t>
+  </si>
+  <si>
+    <t>2012-04</t>
+  </si>
+  <si>
+    <t>2012-05</t>
+  </si>
+  <si>
+    <t>2012-06</t>
+  </si>
+  <si>
+    <t>2012-07</t>
+  </si>
+  <si>
+    <t>2012-08</t>
+  </si>
+  <si>
+    <t>2012-09</t>
+  </si>
+  <si>
+    <t>2012-10</t>
+  </si>
+  <si>
+    <t>2012-11</t>
+  </si>
+  <si>
+    <t>2012-12</t>
+  </si>
+  <si>
+    <t>2013-01</t>
+  </si>
+  <si>
+    <t>2013-02</t>
+  </si>
+  <si>
+    <t>2013-03</t>
+  </si>
+  <si>
+    <t>2013-04</t>
+  </si>
+  <si>
+    <t>2013-05</t>
+  </si>
+  <si>
+    <t>2013-06</t>
+  </si>
+  <si>
+    <t>2013-07</t>
+  </si>
+  <si>
+    <t>2013-08</t>
+  </si>
+  <si>
+    <t>2013-09</t>
+  </si>
+  <si>
+    <t>2013-10</t>
+  </si>
+  <si>
+    <t>2013-11</t>
+  </si>
+  <si>
+    <t>2013-12</t>
+  </si>
+  <si>
+    <t>2014-01</t>
+  </si>
+  <si>
+    <t>2014-02</t>
+  </si>
+  <si>
+    <t>2014-03</t>
+  </si>
+  <si>
+    <t>2014-04</t>
+  </si>
+  <si>
+    <t>2014-05</t>
+  </si>
+  <si>
+    <t>2014-06</t>
+  </si>
+  <si>
+    <t>2014-07</t>
+  </si>
+  <si>
+    <t>2014-08</t>
+  </si>
+  <si>
+    <t>2014-09</t>
+  </si>
+  <si>
+    <t>2014-10</t>
+  </si>
+  <si>
+    <t>2014-11</t>
+  </si>
+  <si>
+    <t>2014-12</t>
+  </si>
+  <si>
+    <t>2015-01</t>
+  </si>
+  <si>
+    <t>2015-02</t>
+  </si>
+  <si>
+    <t>2015-03</t>
+  </si>
+  <si>
+    <t>2015-04</t>
+  </si>
+  <si>
+    <t>2015-05</t>
+  </si>
+  <si>
+    <t>2015-06</t>
+  </si>
+  <si>
+    <t>2016-01</t>
+  </si>
+  <si>
+    <t>2016-02</t>
+  </si>
+  <si>
+    <t>2016-03</t>
+  </si>
+  <si>
+    <t>2016-04</t>
+  </si>
+  <si>
+    <t>2016-05</t>
+  </si>
+  <si>
+    <t>2016-06</t>
+  </si>
+  <si>
+    <t>2016-07</t>
+  </si>
+  <si>
+    <t>2016-08</t>
+  </si>
+  <si>
+    <t>2016-09</t>
+  </si>
+  <si>
+    <t>2016-10</t>
+  </si>
+  <si>
+    <t>2016-11</t>
+  </si>
+  <si>
+    <t>2016-12</t>
+  </si>
+  <si>
+    <t>2017-01</t>
+  </si>
+  <si>
+    <t>2017-02</t>
+  </si>
+  <si>
+    <t>2017-03</t>
+  </si>
+  <si>
+    <t>2017-04</t>
+  </si>
+  <si>
+    <t>2017-05</t>
+  </si>
+  <si>
+    <t>2017-06</t>
+  </si>
+  <si>
+    <t>2017-07</t>
+  </si>
+  <si>
+    <t>2017-08</t>
+  </si>
+  <si>
+    <t>2017-09</t>
+  </si>
+  <si>
+    <t>2017-10</t>
+  </si>
+  <si>
+    <t>2017-11</t>
+  </si>
+  <si>
+    <t>2017-12</t>
+  </si>
+  <si>
+    <t>2018-01</t>
+  </si>
+  <si>
+    <t>2018-02</t>
+  </si>
+  <si>
+    <t>2018-03</t>
+  </si>
+  <si>
+    <t>2018-04</t>
+  </si>
+  <si>
+    <t>2018-05</t>
+  </si>
+  <si>
+    <t>2018-06</t>
+  </si>
+  <si>
+    <t>2018-07</t>
+  </si>
+  <si>
+    <t>2018-08</t>
+  </si>
+  <si>
+    <t>2018-09</t>
+  </si>
+  <si>
+    <t>2018-10</t>
+  </si>
+  <si>
+    <t>2018-11</t>
+  </si>
+  <si>
+    <t>2018-12</t>
+  </si>
+  <si>
+    <t>2019-01</t>
+  </si>
+  <si>
+    <t>2019-02</t>
+  </si>
+  <si>
+    <t>2019-03</t>
+  </si>
+  <si>
+    <t>2019-04</t>
+  </si>
+  <si>
+    <t>2019-05</t>
+  </si>
+  <si>
+    <t>2019-06</t>
+  </si>
+  <si>
+    <t>2019-07</t>
+  </si>
+  <si>
+    <t>2019-08</t>
+  </si>
+  <si>
+    <t>2019-09</t>
+  </si>
+  <si>
+    <t>2019-10</t>
+  </si>
+  <si>
+    <t>2019-11</t>
+  </si>
+  <si>
+    <t>2019-12</t>
+  </si>
+  <si>
+    <t>2015-07</t>
+  </si>
+  <si>
+    <t>2015-08</t>
+  </si>
+  <si>
+    <t>2015-09</t>
+  </si>
+  <si>
+    <t>2015-10</t>
+  </si>
+  <si>
+    <t>2015-11</t>
+  </si>
+  <si>
+    <t>2015-12</t>
   </si>
 </sst>
 </file>
@@ -82,11 +412,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="mmm\-yyyy"/>
     <numFmt numFmtId="165" formatCode="0;\-0;0;@"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="[$-F400]h:mm:ss\ am/pm"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -110,6 +440,12 @@
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -136,13 +472,13 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -481,8 +817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3BF0304-FC47-CD40-9AC3-EF3B234E7ECD}">
   <dimension ref="A1:C121"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="63" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -505,1326 +841,1327 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
-        <v>40179</v>
-      </c>
-      <c r="B2" s="3">
+      <c r="A2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2">
         <v>4406</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>0.89090000000000003</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
-        <v>40210</v>
-      </c>
-      <c r="B3" s="3">
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2">
         <v>3955</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>0.88990000000000002</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
-        <v>40238</v>
-      </c>
-      <c r="B4" s="3">
+      <c r="A4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2">
         <v>4261</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>0.91590000000000005</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
-        <v>40269</v>
-      </c>
-      <c r="B5" s="3">
+      <c r="A5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2">
         <v>5478</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>0.93</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
-        <v>40299</v>
-      </c>
-      <c r="B6" s="3">
+      <c r="A6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2">
         <v>5592</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>0.84899999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
-        <v>40330</v>
-      </c>
-      <c r="B7" s="3">
+      <c r="A7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="2">
         <v>6549</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>0.85229999999999995</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
-        <v>40360</v>
-      </c>
-      <c r="B8" s="3">
+      <c r="A8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2">
         <v>6301</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>0.89859999999999995</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
-        <v>40391</v>
-      </c>
-      <c r="B9" s="3">
+      <c r="A9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="2">
         <v>6781</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>0.89180000000000004</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
-        <v>40422</v>
-      </c>
-      <c r="B10" s="3">
+      <c r="A10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="2">
         <v>5860</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>0.9667</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
-        <v>40452</v>
-      </c>
-      <c r="B11" s="3">
+      <c r="A11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="2">
         <v>5799</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <v>0.97609999999999997</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
-        <v>40483</v>
-      </c>
-      <c r="B12" s="3">
+      <c r="A12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="2">
         <v>5685</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="3">
         <v>0.96179999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
-        <v>40513</v>
-      </c>
-      <c r="B13" s="3">
+      <c r="A13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="2">
         <v>5922</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="3">
         <v>1.0163</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
-        <v>40544</v>
-      </c>
-      <c r="B14" s="3">
+      <c r="A14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="2">
         <v>4461</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="3">
         <v>0.99239999999999995</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
-        <v>40575</v>
-      </c>
-      <c r="B15" s="3">
+      <c r="A15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="2">
         <v>4371</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="3">
         <v>1.0163</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
-        <v>40603</v>
-      </c>
-      <c r="B16" s="3">
+      <c r="A16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="2">
         <v>5447</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="3">
         <v>1.0334000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
-        <v>40634</v>
-      </c>
-      <c r="B17" s="3">
+      <c r="A17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="2">
         <v>5744</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="3">
         <v>1.0900000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
-        <v>40664</v>
-      </c>
-      <c r="B18" s="3">
+      <c r="A18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="2">
         <v>6074</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="3">
         <v>1.0709</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
-        <v>40695</v>
-      </c>
-      <c r="B19" s="3">
+      <c r="A19" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="2">
         <v>6721</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="3">
         <v>1.0739000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
-        <v>40725</v>
-      </c>
-      <c r="B20" s="3">
+      <c r="A20" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="2">
         <v>6231</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="3">
         <v>1.0953999999999999</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
-        <v>40756</v>
-      </c>
-      <c r="B21" s="3">
+      <c r="A21" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="2">
         <v>7275</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="3">
         <v>1.0690999999999999</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="2">
-        <v>40787</v>
-      </c>
-      <c r="B22" s="3">
+      <c r="A22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="2">
         <v>6635</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="3">
         <v>0.97809999999999997</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="2">
-        <v>40817</v>
-      </c>
-      <c r="B23" s="3">
+      <c r="A23" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="2">
         <v>6763</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23" s="3">
         <v>1.0508999999999999</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="2">
-        <v>40848</v>
-      </c>
-      <c r="B24" s="3">
+      <c r="A24" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="2">
         <v>6469</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24" s="3">
         <v>1.0021</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="2">
-        <v>40878</v>
-      </c>
-      <c r="B25" s="3">
+      <c r="A25" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="2">
         <v>7203</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C25" s="3">
         <v>1.0156000000000001</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="2">
-        <v>40909</v>
-      </c>
-      <c r="B26" s="3">
+      <c r="A26" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="2">
         <v>6236</v>
       </c>
-      <c r="C26" s="4">
+      <c r="C26" s="3">
         <v>1.0637000000000001</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="2">
-        <v>40940</v>
-      </c>
-      <c r="B27" s="3">
+      <c r="A27" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="2">
         <v>5141</v>
       </c>
-      <c r="C27" s="4">
+      <c r="C27" s="3">
         <v>1.0815999999999999</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="2">
-        <v>40969</v>
-      </c>
-      <c r="B28" s="3">
+      <c r="A28" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="2">
         <v>5724</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C28" s="3">
         <v>1.0402</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="2">
-        <v>41000</v>
-      </c>
-      <c r="B29" s="3">
+      <c r="A29" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="2">
         <v>5819</v>
       </c>
-      <c r="C29" s="4">
+      <c r="C29" s="3">
         <v>1.0452999999999999</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="2">
-        <v>41030</v>
-      </c>
-      <c r="B30" s="3">
+      <c r="A30" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="2">
         <v>5833</v>
       </c>
-      <c r="C30" s="4">
+      <c r="C30" s="3">
         <v>0.97270000000000001</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="2">
-        <v>41061</v>
-      </c>
-      <c r="B31" s="3">
+      <c r="A31" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" s="2">
         <v>6189</v>
       </c>
-      <c r="C31" s="4">
+      <c r="C31" s="3">
         <v>1.0190999999999999</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="2">
-        <v>41091</v>
-      </c>
-      <c r="B32" s="3">
+      <c r="A32" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" s="2">
         <v>6326</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32" s="3">
         <v>1.0526</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="2">
-        <v>41122</v>
-      </c>
-      <c r="B33" s="3">
+      <c r="A33" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" s="2">
         <v>6098</v>
       </c>
-      <c r="C33" s="4">
+      <c r="C33" s="3">
         <v>1.0301</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="2">
-        <v>41153</v>
-      </c>
-      <c r="B34" s="3">
+      <c r="A34" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="2">
         <v>5880</v>
       </c>
-      <c r="C34" s="4">
+      <c r="C34" s="3">
         <v>1.0464</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="2">
-        <v>41183</v>
-      </c>
-      <c r="B35" s="3">
+      <c r="A35" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" s="2">
         <v>5781</v>
       </c>
-      <c r="C35" s="4">
+      <c r="C35" s="3">
         <v>1.0378000000000001</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="2">
-        <v>41214</v>
-      </c>
-      <c r="B36" s="3">
+      <c r="A36" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" s="2">
         <v>5426</v>
       </c>
-      <c r="C36" s="4">
+      <c r="C36" s="3">
         <v>1.0430999999999999</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="2">
-        <v>41244</v>
-      </c>
-      <c r="B37" s="3">
+      <c r="A37" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" s="2">
         <v>5891</v>
       </c>
-      <c r="C37" s="4">
+      <c r="C37" s="3">
         <v>1.0384</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="2">
-        <v>41275</v>
-      </c>
-      <c r="B38" s="3">
+      <c r="A38" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38" s="2">
         <v>5222</v>
       </c>
-      <c r="C38" s="4">
+      <c r="C38" s="3">
         <v>1.0394000000000001</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="2">
-        <v>41306</v>
-      </c>
-      <c r="B39" s="3">
+      <c r="A39" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" s="2">
         <v>4587</v>
       </c>
-      <c r="C39" s="4">
+      <c r="C39" s="3">
         <v>1.0275000000000001</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="2">
-        <v>41334</v>
-      </c>
-      <c r="B40" s="3">
+      <c r="A40" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" s="2">
         <v>5159</v>
       </c>
-      <c r="C40" s="4">
+      <c r="C40" s="3">
         <v>1.0426</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="2">
-        <v>41365</v>
-      </c>
-      <c r="B41" s="3">
+      <c r="A41" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" s="2">
         <v>5090</v>
       </c>
-      <c r="C41" s="4">
+      <c r="C41" s="3">
         <v>1.0367999999999999</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="2">
-        <v>41395</v>
-      </c>
-      <c r="B42" s="3">
+      <c r="A42" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B42" s="2">
         <v>5635</v>
       </c>
-      <c r="C42" s="4">
+      <c r="C42" s="3">
         <v>0.96489999999999998</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="2">
-        <v>41426</v>
-      </c>
-      <c r="B43" s="3">
+      <c r="A43" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43" s="2">
         <v>5849</v>
       </c>
-      <c r="C43" s="4">
+      <c r="C43" s="3">
         <v>0.92749999999999999</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="2">
-        <v>41456</v>
-      </c>
-      <c r="B44" s="3">
+      <c r="A44" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B44" s="2">
         <v>6220</v>
       </c>
-      <c r="C44" s="4">
+      <c r="C44" s="3">
         <v>0.90369999999999995</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="2">
-        <v>41487</v>
-      </c>
-      <c r="B45" s="3">
+      <c r="A45" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45" s="2">
         <v>6030</v>
       </c>
-      <c r="C45" s="4">
+      <c r="C45" s="3">
         <v>0.89470000000000005</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="2">
-        <v>41518</v>
-      </c>
-      <c r="B46" s="3">
+      <c r="A46" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B46" s="2">
         <v>5743</v>
       </c>
-      <c r="C46" s="4">
+      <c r="C46" s="3">
         <v>0.93089999999999995</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="2">
-        <v>41548</v>
-      </c>
-      <c r="B47" s="3">
+      <c r="A47" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B47" s="2">
         <v>5784</v>
       </c>
-      <c r="C47" s="4">
+      <c r="C47" s="3">
         <v>0.94899999999999995</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="2">
-        <v>41579</v>
-      </c>
-      <c r="B48" s="3">
+      <c r="A48" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B48" s="2">
         <v>5534</v>
       </c>
-      <c r="C48" s="4">
+      <c r="C48" s="3">
         <v>0.90869999999999995</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="2">
-        <v>41609</v>
-      </c>
-      <c r="B49" s="3">
+      <c r="A49" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B49" s="2">
         <v>6660</v>
       </c>
-      <c r="C49" s="4">
+      <c r="C49" s="3">
         <v>0.89480000000000004</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="2">
-        <v>41640</v>
-      </c>
-      <c r="B50" s="3">
+      <c r="A50" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B50" s="2">
         <v>6157</v>
       </c>
-      <c r="C50" s="4">
+      <c r="C50" s="3">
         <v>0.87629999999999997</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="2">
-        <v>41671</v>
-      </c>
-      <c r="B51" s="3">
+      <c r="A51" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B51" s="2">
         <v>5695</v>
       </c>
-      <c r="C51" s="4">
+      <c r="C51" s="3">
         <v>0.89470000000000005</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="2">
-        <v>41699</v>
-      </c>
-      <c r="B52" s="3">
+      <c r="A52" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B52" s="2">
         <v>6073</v>
       </c>
-      <c r="C52" s="4">
+      <c r="C52" s="3">
         <v>0.92210000000000003</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="2">
-        <v>41730</v>
-      </c>
-      <c r="B53" s="3">
+      <c r="A53" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B53" s="2">
         <v>5723</v>
       </c>
-      <c r="C53" s="4">
+      <c r="C53" s="3">
         <v>0.92869999999999997</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" s="2">
-        <v>41760</v>
-      </c>
-      <c r="B54" s="3">
+      <c r="A54" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B54" s="2">
         <v>5415</v>
       </c>
-      <c r="C54" s="4">
+      <c r="C54" s="3">
         <v>0.93189999999999995</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="2">
-        <v>41791</v>
-      </c>
-      <c r="B55" s="3">
+      <c r="A55" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B55" s="2">
         <v>5954</v>
       </c>
-      <c r="C55" s="4">
+      <c r="C55" s="3">
         <v>0.94199999999999995</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" s="2">
-        <v>41821</v>
-      </c>
-      <c r="B56" s="3">
+      <c r="A56" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B56" s="2">
         <v>6065</v>
       </c>
-      <c r="C56" s="4">
+      <c r="C56" s="3">
         <v>0.93240000000000001</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="2">
-        <v>41852</v>
-      </c>
-      <c r="B57" s="3">
+      <c r="A57" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B57" s="2">
         <v>5730</v>
       </c>
-      <c r="C57" s="4">
+      <c r="C57" s="3">
         <v>0.93489999999999995</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" s="2">
-        <v>41883</v>
-      </c>
-      <c r="B58" s="3">
+      <c r="A58" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B58" s="2">
         <v>5691</v>
       </c>
-      <c r="C58" s="4">
+      <c r="C58" s="3">
         <v>0.87519999999999998</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" s="2">
-        <v>41913</v>
-      </c>
-      <c r="B59" s="3">
+      <c r="A59" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B59" s="2">
         <v>5828</v>
       </c>
-      <c r="C59" s="4">
+      <c r="C59" s="3">
         <v>0.88049999999999995</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" s="2">
-        <v>41944</v>
-      </c>
-      <c r="B60" s="3">
+      <c r="A60" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B60" s="2">
         <v>6033</v>
       </c>
-      <c r="C60" s="4">
+      <c r="C60" s="3">
         <v>0.84909999999999997</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" s="2">
-        <v>41974</v>
-      </c>
-      <c r="B61" s="3">
+      <c r="A61" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B61" s="2">
         <v>6147</v>
       </c>
-      <c r="C61" s="4">
+      <c r="C61" s="3">
         <v>0.82020000000000004</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" s="2">
-        <v>42005</v>
-      </c>
-      <c r="B62" s="3">
+      <c r="A62" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B62" s="2">
         <v>5785</v>
       </c>
-      <c r="C62" s="4">
+      <c r="C62" s="3">
         <v>0.77810000000000001</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" s="2">
-        <v>42036</v>
-      </c>
-      <c r="B63" s="3">
+      <c r="A63" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B63" s="2">
         <v>5318</v>
       </c>
-      <c r="C63" s="4">
+      <c r="C63" s="3">
         <v>0.7792</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" s="2">
-        <v>42064</v>
-      </c>
-      <c r="B64" s="3">
+      <c r="A64" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B64" s="2">
         <v>5527</v>
       </c>
-      <c r="C64" s="4">
+      <c r="C64" s="3">
         <v>0.76339999999999997</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65" s="2">
-        <v>42095</v>
-      </c>
-      <c r="B65" s="3">
+      <c r="A65" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B65" s="2">
         <v>4699</v>
       </c>
-      <c r="C65" s="4">
+      <c r="C65" s="3">
         <v>0.79810000000000003</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" s="2">
-        <v>42125</v>
-      </c>
-      <c r="B66" s="3">
+      <c r="A66" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B66" s="2">
         <v>4458</v>
       </c>
-      <c r="C66" s="4">
+      <c r="C66" s="3">
         <v>0.76629999999999998</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" s="2">
-        <v>42156</v>
-      </c>
-      <c r="B67" s="3">
+      <c r="A67" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B67" s="2">
         <v>5155</v>
       </c>
-      <c r="C67" s="4">
+      <c r="C67" s="3">
         <v>0.76800000000000002</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" s="2">
-        <v>42186</v>
-      </c>
-      <c r="B68" s="3">
+      <c r="A68" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B68" s="2">
         <v>5256</v>
       </c>
-      <c r="C68" s="4">
+      <c r="C68" s="3">
         <v>0.72940000000000005</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69" s="2">
-        <v>42217</v>
-      </c>
-      <c r="B69" s="3">
+      <c r="A69" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B69" s="2">
         <v>5578</v>
       </c>
-      <c r="C69" s="4">
+      <c r="C69" s="3">
         <v>0.71489999999999998</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" s="2">
-        <v>42248</v>
-      </c>
-      <c r="B70" s="3">
+      <c r="A70" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B70" s="2">
         <v>5189</v>
       </c>
-      <c r="C70" s="4">
+      <c r="C70" s="3">
         <v>0.70099999999999996</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" s="2">
-        <v>42278</v>
-      </c>
-      <c r="B71" s="3">
+      <c r="A71" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B71" s="2">
         <v>5163</v>
       </c>
-      <c r="C71" s="4">
+      <c r="C71" s="3">
         <v>0.70989999999999998</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" s="2">
-        <v>42309</v>
-      </c>
-      <c r="B72" s="3">
+      <c r="A72" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B72" s="2">
         <v>5125</v>
       </c>
-      <c r="C72" s="4">
+      <c r="C72" s="3">
         <v>0.71889999999999998</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73" s="2">
-        <v>42339</v>
-      </c>
-      <c r="B73" s="3">
+      <c r="A73" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B73" s="2">
         <v>4995</v>
       </c>
-      <c r="C73" s="4">
+      <c r="C73" s="3">
         <v>0.73060000000000003</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74" s="2">
-        <v>42370</v>
-      </c>
-      <c r="B74" s="3">
+      <c r="A74" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B74" s="2">
         <v>4777</v>
       </c>
-      <c r="C74" s="4">
+      <c r="C74" s="3">
         <v>0.71</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A75" s="2">
-        <v>42401</v>
-      </c>
-      <c r="B75" s="3">
+      <c r="A75" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B75" s="2">
         <v>4347</v>
       </c>
-      <c r="C75" s="4">
+      <c r="C75" s="3">
         <v>0.71399999999999997</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A76" s="2">
-        <v>42430</v>
-      </c>
-      <c r="B76" s="3">
+      <c r="A76" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B76" s="2">
         <v>4675</v>
       </c>
-      <c r="C76" s="4">
+      <c r="C76" s="3">
         <v>0.76570000000000005</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A77" s="2">
-        <v>42461</v>
-      </c>
-      <c r="B77" s="3">
+      <c r="A77" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B77" s="2">
         <v>4335</v>
       </c>
-      <c r="C77" s="4">
+      <c r="C77" s="3">
         <v>0.76549999999999996</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A78" s="2">
-        <v>42491</v>
-      </c>
-      <c r="B78" s="3">
+      <c r="A78" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B78" s="2">
         <v>4490</v>
       </c>
-      <c r="C78" s="4">
+      <c r="C78" s="3">
         <v>0.72419999999999995</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A79" s="2">
-        <v>42522</v>
-      </c>
-      <c r="B79" s="3">
+      <c r="A79" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B79" s="2">
         <v>4888</v>
       </c>
-      <c r="C79" s="4">
+      <c r="C79" s="3">
         <v>0.74260000000000004</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A80" s="2">
-        <v>42552</v>
-      </c>
-      <c r="B80" s="3">
+      <c r="A80" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B80" s="2">
         <v>4886</v>
       </c>
-      <c r="C80" s="4">
+      <c r="C80" s="3">
         <v>0.75219999999999998</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A81" s="2">
-        <v>42583</v>
-      </c>
-      <c r="B81" s="3">
+      <c r="A81" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B81" s="2">
         <v>5288</v>
       </c>
-      <c r="C81" s="4">
+      <c r="C81" s="3">
         <v>0.75139999999999996</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A82" s="2">
-        <v>42614</v>
-      </c>
-      <c r="B82" s="3">
+      <c r="A82" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B82" s="2">
         <v>5750</v>
       </c>
-      <c r="C82" s="4">
+      <c r="C82" s="3">
         <v>0.76300000000000001</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A83" s="2">
-        <v>42644</v>
-      </c>
-      <c r="B83" s="3">
+      <c r="A83" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B83" s="2">
         <v>6523</v>
       </c>
-      <c r="C83" s="4">
+      <c r="C83" s="3">
         <v>0.76129999999999998</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A84" s="2">
-        <v>42675</v>
-      </c>
-      <c r="B84" s="3">
+      <c r="A84" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B84" s="2">
         <v>8193</v>
       </c>
-      <c r="C84" s="4">
+      <c r="C84" s="3">
         <v>0.74739999999999995</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A85" s="2">
-        <v>42705</v>
-      </c>
-      <c r="B85" s="3">
+      <c r="A85" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B85" s="2">
         <v>9550</v>
       </c>
-      <c r="C85" s="4">
+      <c r="C85" s="3">
         <v>0.72360000000000002</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A86" s="2">
-        <v>42736</v>
-      </c>
-      <c r="B86" s="3">
+      <c r="A86" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B86" s="2">
         <v>7948</v>
       </c>
-      <c r="C86" s="4">
+      <c r="C86" s="3">
         <v>0.75670000000000004</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A87" s="2">
-        <v>42767</v>
-      </c>
-      <c r="B87" s="3">
+      <c r="A87" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B87" s="2">
         <v>7133</v>
       </c>
-      <c r="C87" s="4">
+      <c r="C87" s="3">
         <v>0.76880000000000004</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A88" s="2">
-        <v>42795</v>
-      </c>
-      <c r="B88" s="3">
+      <c r="A88" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B88" s="2">
         <v>7588</v>
       </c>
-      <c r="C88" s="4">
+      <c r="C88" s="3">
         <v>0.76439999999999997</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A89" s="2">
-        <v>42826</v>
-      </c>
-      <c r="B89" s="3">
+      <c r="A89" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B89" s="2">
         <v>5411</v>
       </c>
-      <c r="C89" s="4">
+      <c r="C89" s="3">
         <v>0.74750000000000005</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A90" s="2">
-        <v>42856</v>
-      </c>
-      <c r="B90" s="3">
+      <c r="A90" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B90" s="2">
         <v>8230</v>
       </c>
-      <c r="C90" s="4">
+      <c r="C90" s="3">
         <v>0.745</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A91" s="2">
-        <v>42887</v>
-      </c>
-      <c r="B91" s="3">
+      <c r="A91" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B91" s="2">
         <v>8207</v>
       </c>
-      <c r="C91" s="4">
+      <c r="C91" s="3">
         <v>0.76919999999999999</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A92" s="2">
-        <v>42917</v>
-      </c>
-      <c r="B92" s="3">
+      <c r="A92" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B92" s="2">
         <v>7671</v>
       </c>
-      <c r="C92" s="4">
+      <c r="C92" s="3">
         <v>0.79869999999999997</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A93" s="2">
-        <v>42948</v>
-      </c>
-      <c r="B93" s="3">
+      <c r="A93" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B93" s="2">
         <v>7618</v>
       </c>
-      <c r="C93" s="4">
+      <c r="C93" s="3">
         <v>0.78979999999999995</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A94" s="2">
-        <v>42979</v>
-      </c>
-      <c r="B94" s="3">
+      <c r="A94" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B94" s="2">
         <v>7548</v>
       </c>
-      <c r="C94" s="4">
+      <c r="C94" s="3">
         <v>0.78390000000000004</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A95" s="2">
-        <v>43009</v>
-      </c>
-      <c r="B95" s="3">
+      <c r="A95" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B95" s="2">
         <v>7446</v>
       </c>
-      <c r="C95" s="4">
+      <c r="C95" s="3">
         <v>0.76729999999999998</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A96" s="2">
-        <v>43040</v>
-      </c>
-      <c r="B96" s="3">
+      <c r="A96" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B96" s="2">
         <v>7738</v>
       </c>
-      <c r="C96" s="4">
+      <c r="C96" s="3">
         <v>0.75849999999999995</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A97" s="2">
-        <v>43070</v>
-      </c>
-      <c r="B97" s="3">
+      <c r="A97" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B97" s="2">
         <v>8611</v>
       </c>
-      <c r="C97" s="4">
+      <c r="C97" s="3">
         <v>0.78</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A98" s="2">
-        <v>43101</v>
-      </c>
-      <c r="B98" s="3">
+      <c r="A98" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B98" s="2">
         <v>9076</v>
       </c>
-      <c r="C98" s="4">
+      <c r="C98" s="3">
         <v>0.80730000000000002</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A99" s="2">
-        <v>43132</v>
-      </c>
-      <c r="B99" s="3">
+      <c r="A99" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B99" s="2">
         <v>8344</v>
       </c>
-      <c r="C99" s="4">
+      <c r="C99" s="3">
         <v>0.7792</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A100" s="2">
-        <v>43160</v>
-      </c>
-      <c r="B100" s="3">
+      <c r="A100" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B100" s="2">
         <v>9252</v>
       </c>
-      <c r="C100" s="4">
+      <c r="C100" s="3">
         <v>0.76649999999999996</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A101" s="2">
-        <v>43191</v>
-      </c>
-      <c r="B101" s="3">
+      <c r="A101" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B101" s="2">
         <v>8575</v>
       </c>
-      <c r="C101" s="4">
+      <c r="C101" s="3">
         <v>0.75700000000000001</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A102" s="2">
-        <v>43221</v>
-      </c>
-      <c r="B102" s="3">
+      <c r="A102" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B102" s="2">
         <v>9219</v>
       </c>
-      <c r="C102" s="4">
+      <c r="C102" s="3">
         <v>0.75639999999999996</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A103" s="2">
-        <v>43252</v>
-      </c>
-      <c r="B103" s="3">
+      <c r="A103" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B103" s="2">
         <v>10173</v>
       </c>
-      <c r="C103" s="4">
+      <c r="C103" s="3">
         <v>0.73909999999999998</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A104" s="2">
-        <v>43282</v>
-      </c>
-      <c r="B104" s="3">
+      <c r="A104" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B104" s="2">
         <v>10602</v>
       </c>
-      <c r="C104" s="4">
+      <c r="C104" s="3">
         <v>0.74309999999999998</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A105" s="2">
-        <v>43313</v>
-      </c>
-      <c r="B105" s="3">
+      <c r="A105" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B105" s="2">
         <v>10875</v>
       </c>
-      <c r="C105" s="4">
+      <c r="C105" s="3">
         <v>0.72599999999999998</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A106" s="2">
-        <v>43344</v>
-      </c>
-      <c r="B106" s="3">
+      <c r="A106" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B106" s="2">
         <v>10748</v>
       </c>
-      <c r="C106" s="4">
+      <c r="C106" s="3">
         <v>0.72219999999999995</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A107" s="2">
-        <v>43374</v>
-      </c>
-      <c r="B107" s="3">
+      <c r="A107" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B107" s="2">
         <v>11983</v>
       </c>
-      <c r="C107" s="4">
+      <c r="C107" s="3">
         <v>0.70850000000000002</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A108" s="2">
-        <v>43405</v>
-      </c>
-      <c r="B108" s="3">
+      <c r="A108" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B108" s="2">
         <v>11581</v>
       </c>
-      <c r="C108" s="4">
+      <c r="C108" s="3">
         <v>0.73160000000000003</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A109" s="2">
-        <v>43435</v>
-      </c>
-      <c r="B109" s="3">
+      <c r="A109" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B109" s="2">
         <v>11841</v>
       </c>
-      <c r="C109" s="4">
+      <c r="C109" s="3">
         <v>0.70579999999999998</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A110" s="2">
-        <v>43466</v>
-      </c>
-      <c r="B110" s="3">
+      <c r="A110" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B110" s="2">
         <v>11710</v>
       </c>
-      <c r="C110" s="4">
+      <c r="C110" s="3">
         <v>0.7268</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A111" s="2">
-        <v>43497</v>
-      </c>
-      <c r="B111" s="3">
+      <c r="A111" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B111" s="2">
         <v>9632</v>
       </c>
-      <c r="C111" s="4">
+      <c r="C111" s="3">
         <v>0.71460000000000001</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A112" s="2">
-        <v>43525</v>
-      </c>
-      <c r="B112" s="3">
+      <c r="A112" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B112" s="2">
         <v>11030</v>
       </c>
-      <c r="C112" s="4">
+      <c r="C112" s="3">
         <v>0.7087</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A113" s="2">
-        <v>43556</v>
-      </c>
-      <c r="B113" s="3">
+      <c r="A113" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B113" s="2">
         <v>10263</v>
       </c>
-      <c r="C113" s="4">
+      <c r="C113" s="3">
         <v>0.70389999999999997</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A114" s="2">
-        <v>43586</v>
-      </c>
-      <c r="B114" s="3">
+      <c r="A114" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B114" s="2">
         <v>10488</v>
       </c>
-      <c r="C114" s="4">
+      <c r="C114" s="3">
         <v>0.69159999999999999</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A115" s="2">
-        <v>43617</v>
-      </c>
-      <c r="B115" s="3">
+      <c r="A115" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B115" s="2">
         <v>11193</v>
       </c>
-      <c r="C115" s="4">
+      <c r="C115" s="3">
         <v>0.70130000000000003</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A116" s="2">
-        <v>43647</v>
-      </c>
-      <c r="B116" s="3">
+      <c r="A116" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B116" s="2">
         <v>10807</v>
       </c>
-      <c r="C116" s="4">
+      <c r="C116" s="3">
         <v>0.68940000000000001</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A117" s="2">
-        <v>43678</v>
-      </c>
-      <c r="B117" s="3">
+      <c r="A117" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B117" s="2">
         <v>11022</v>
       </c>
-      <c r="C117" s="4">
+      <c r="C117" s="3">
         <v>0.67179999999999995</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A118" s="2">
-        <v>43709</v>
-      </c>
-      <c r="B118" s="3">
+      <c r="A118" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B118" s="2">
         <v>10176</v>
       </c>
-      <c r="C118" s="4">
+      <c r="C118" s="3">
         <v>0.67490000000000006</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A119" s="2">
-        <v>43739</v>
-      </c>
-      <c r="B119" s="3">
+      <c r="A119" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B119" s="2">
         <v>9781</v>
       </c>
-      <c r="C119" s="4">
+      <c r="C119" s="3">
         <v>0.69259999999999999</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A120" s="2">
-        <v>43770</v>
-      </c>
-      <c r="B120" s="3">
+      <c r="A120" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B120" s="2">
         <v>9755</v>
       </c>
-      <c r="C120" s="4">
+      <c r="C120" s="3">
         <v>0.67769999999999997</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A121" s="2">
-        <v>43800</v>
-      </c>
-      <c r="B121" s="3">
+      <c r="A121" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B121" s="2">
         <v>10385</v>
       </c>
-      <c r="C121" s="4">
+      <c r="C121" s="3">
         <v>0.7006</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>